<commit_message>
temporary (network of yolov4-csp, yolov4x-mish is wrong)
</commit_message>
<xml_diff>
--- a/tools/yolov4x-mish.xlsx
+++ b/tools/yolov4x-mish.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maruyama/Projects/private/public/yolo_various_platforms/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{85316376-EE9F-3A4B-9BF2-DB3EC18CCC77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98D3AB2-AC9C-A842-AE15-34637232C2B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="500" windowWidth="27900" windowHeight="16940"/>
+    <workbookView xWindow="8060" yWindow="19020" windowWidth="18920" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="yolov4x-mish" sheetId="1" r:id="rId1"/>
@@ -218,26 +218,26 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>concat(x, x_57)</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>x → x_57</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>concat(x, x_94)</t>
     <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>x → x_94</t>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>concat(x, x_135)</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>concat(x, x_151)</t>
+    <phoneticPr fontId="18"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -877,6 +877,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -885,18 +897,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1252,11 +1252,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="P193" sqref="P193"/>
+    <sheetView tabSelected="1" topLeftCell="F125" workbookViewId="0">
+      <selection activeCell="L157" sqref="L157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -1340,7 +1340,7 @@
         <v>44</v>
       </c>
       <c r="M2" s="4"/>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1375,7 +1375,7 @@
       <c r="L3" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N3" s="4"/>
@@ -1408,7 +1408,7 @@
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M4" s="4"/>
@@ -1442,7 +1442,7 @@
       <c r="I5">
         <v>3</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
@@ -1459,7 +1459,7 @@
       <c r="J6">
         <v>-3</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
@@ -1494,7 +1494,7 @@
       <c r="L7" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N7" s="4"/>
@@ -1611,7 +1611,7 @@
       <c r="I11">
         <v>9</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M11" s="4"/>
@@ -1645,7 +1645,7 @@
       <c r="I12">
         <v>10</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="6"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
@@ -1662,7 +1662,7 @@
       <c r="J13">
         <v>-3</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
@@ -1694,7 +1694,7 @@
       <c r="I14">
         <v>12</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M14" s="4"/>
@@ -1728,7 +1728,7 @@
       <c r="I15">
         <v>13</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="6"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
     </row>
@@ -1745,7 +1745,7 @@
       <c r="J16">
         <v>-3</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="7"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
     </row>
@@ -1777,7 +1777,7 @@
       <c r="I17">
         <v>15</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M17" s="4"/>
@@ -1811,7 +1811,7 @@
       <c r="I18">
         <v>16</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
     </row>
@@ -1828,7 +1828,7 @@
       <c r="J19">
         <v>-3</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="7"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
     </row>
@@ -1947,7 +1947,7 @@
       <c r="L23" t="s">
         <v>35</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N23" s="4"/>
@@ -2064,7 +2064,7 @@
       <c r="I27">
         <v>25</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L27" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M27" s="4"/>
@@ -2098,7 +2098,7 @@
       <c r="I28">
         <v>26</v>
       </c>
-      <c r="L28" s="2"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
     </row>
@@ -2115,7 +2115,7 @@
       <c r="J29">
         <v>-3</v>
       </c>
-      <c r="L29" s="3"/>
+      <c r="L29" s="7"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
     </row>
@@ -2147,7 +2147,7 @@
       <c r="I30">
         <v>28</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L30" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M30" s="4"/>
@@ -2181,7 +2181,7 @@
       <c r="I31">
         <v>29</v>
       </c>
-      <c r="L31" s="2"/>
+      <c r="L31" s="6"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
     </row>
@@ -2198,7 +2198,7 @@
       <c r="J32">
         <v>-3</v>
       </c>
-      <c r="L32" s="3"/>
+      <c r="L32" s="7"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
     </row>
@@ -2230,7 +2230,7 @@
       <c r="I33">
         <v>31</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="L33" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M33" s="4"/>
@@ -2264,7 +2264,7 @@
       <c r="I34">
         <v>32</v>
       </c>
-      <c r="L34" s="2"/>
+      <c r="L34" s="6"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
     </row>
@@ -2281,7 +2281,7 @@
       <c r="J35">
         <v>-3</v>
       </c>
-      <c r="L35" s="3"/>
+      <c r="L35" s="7"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
     </row>
@@ -2313,7 +2313,7 @@
       <c r="I36">
         <v>34</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="L36" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M36" s="4"/>
@@ -2347,7 +2347,7 @@
       <c r="I37">
         <v>35</v>
       </c>
-      <c r="L37" s="2"/>
+      <c r="L37" s="6"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
@@ -2364,7 +2364,7 @@
       <c r="J38">
         <v>-3</v>
       </c>
-      <c r="L38" s="3"/>
+      <c r="L38" s="7"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
@@ -2396,7 +2396,7 @@
       <c r="I39">
         <v>37</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="L39" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M39" s="4"/>
@@ -2430,7 +2430,7 @@
       <c r="I40">
         <v>38</v>
       </c>
-      <c r="L40" s="2"/>
+      <c r="L40" s="6"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
@@ -2447,7 +2447,7 @@
       <c r="J41">
         <v>-3</v>
       </c>
-      <c r="L41" s="3"/>
+      <c r="L41" s="7"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
@@ -2479,7 +2479,7 @@
       <c r="I42">
         <v>40</v>
       </c>
-      <c r="L42" s="1" t="s">
+      <c r="L42" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M42" s="4"/>
@@ -2513,7 +2513,7 @@
       <c r="I43">
         <v>41</v>
       </c>
-      <c r="L43" s="2"/>
+      <c r="L43" s="6"/>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
     </row>
@@ -2530,7 +2530,7 @@
       <c r="J44">
         <v>-3</v>
       </c>
-      <c r="L44" s="3"/>
+      <c r="L44" s="7"/>
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
     </row>
@@ -2562,7 +2562,7 @@
       <c r="I45">
         <v>43</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="L45" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M45" s="4"/>
@@ -2596,7 +2596,7 @@
       <c r="I46">
         <v>44</v>
       </c>
-      <c r="L46" s="2"/>
+      <c r="L46" s="6"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
     </row>
@@ -2613,7 +2613,7 @@
       <c r="J47">
         <v>-3</v>
       </c>
-      <c r="L47" s="3"/>
+      <c r="L47" s="7"/>
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
     </row>
@@ -2645,7 +2645,7 @@
       <c r="I48">
         <v>46</v>
       </c>
-      <c r="L48" s="1" t="s">
+      <c r="L48" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M48" s="4"/>
@@ -2679,7 +2679,7 @@
       <c r="I49">
         <v>47</v>
       </c>
-      <c r="L49" s="2"/>
+      <c r="L49" s="6"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
     </row>
@@ -2696,7 +2696,7 @@
       <c r="J50">
         <v>-3</v>
       </c>
-      <c r="L50" s="3"/>
+      <c r="L50" s="7"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
     </row>
@@ -2728,7 +2728,7 @@
       <c r="I51">
         <v>49</v>
       </c>
-      <c r="L51" s="1" t="s">
+      <c r="L51" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M51" s="4"/>
@@ -2762,7 +2762,7 @@
       <c r="I52">
         <v>50</v>
       </c>
-      <c r="L52" s="2"/>
+      <c r="L52" s="6"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
     </row>
@@ -2779,7 +2779,7 @@
       <c r="J53">
         <v>-3</v>
       </c>
-      <c r="L53" s="3"/>
+      <c r="L53" s="7"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
     </row>
@@ -2811,7 +2811,7 @@
       <c r="I54">
         <v>52</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L54" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M54" s="4"/>
@@ -2845,7 +2845,7 @@
       <c r="I55">
         <v>53</v>
       </c>
-      <c r="L55" s="2"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
@@ -2862,7 +2862,7 @@
       <c r="J56">
         <v>-3</v>
       </c>
-      <c r="L56" s="3"/>
+      <c r="L56" s="7"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
     </row>
@@ -2941,7 +2941,7 @@
       <c r="H59">
         <v>1</v>
       </c>
-      <c r="I59" s="7">
+      <c r="I59" s="2">
         <v>57</v>
       </c>
       <c r="L59" t="s">
@@ -2981,7 +2981,7 @@
       <c r="L60" t="s">
         <v>35</v>
       </c>
-      <c r="M60" s="5" t="s">
+      <c r="M60" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N60" s="4"/>
@@ -3098,7 +3098,7 @@
       <c r="I64">
         <v>62</v>
       </c>
-      <c r="L64" s="1" t="s">
+      <c r="L64" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M64" s="4"/>
@@ -3132,7 +3132,7 @@
       <c r="I65">
         <v>63</v>
       </c>
-      <c r="L65" s="2"/>
+      <c r="L65" s="6"/>
       <c r="M65" s="4"/>
       <c r="N65" s="4"/>
     </row>
@@ -3149,7 +3149,7 @@
       <c r="J66">
         <v>-3</v>
       </c>
-      <c r="L66" s="3"/>
+      <c r="L66" s="7"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
     </row>
@@ -3181,7 +3181,7 @@
       <c r="I67">
         <v>65</v>
       </c>
-      <c r="L67" s="1" t="s">
+      <c r="L67" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M67" s="4"/>
@@ -3215,7 +3215,7 @@
       <c r="I68">
         <v>66</v>
       </c>
-      <c r="L68" s="2"/>
+      <c r="L68" s="6"/>
       <c r="M68" s="4"/>
       <c r="N68" s="4"/>
     </row>
@@ -3232,7 +3232,7 @@
       <c r="J69">
         <v>-3</v>
       </c>
-      <c r="L69" s="3"/>
+      <c r="L69" s="7"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
     </row>
@@ -3264,7 +3264,7 @@
       <c r="I70">
         <v>68</v>
       </c>
-      <c r="L70" s="1" t="s">
+      <c r="L70" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M70" s="4"/>
@@ -3298,7 +3298,7 @@
       <c r="I71">
         <v>69</v>
       </c>
-      <c r="L71" s="2"/>
+      <c r="L71" s="6"/>
       <c r="M71" s="4"/>
       <c r="N71" s="4"/>
     </row>
@@ -3315,7 +3315,7 @@
       <c r="J72">
         <v>-3</v>
       </c>
-      <c r="L72" s="3"/>
+      <c r="L72" s="7"/>
       <c r="M72" s="4"/>
       <c r="N72" s="4"/>
     </row>
@@ -3347,7 +3347,7 @@
       <c r="I73">
         <v>71</v>
       </c>
-      <c r="L73" s="1" t="s">
+      <c r="L73" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M73" s="4"/>
@@ -3381,7 +3381,7 @@
       <c r="I74">
         <v>72</v>
       </c>
-      <c r="L74" s="2"/>
+      <c r="L74" s="6"/>
       <c r="M74" s="4"/>
       <c r="N74" s="4"/>
     </row>
@@ -3398,7 +3398,7 @@
       <c r="J75">
         <v>-3</v>
       </c>
-      <c r="L75" s="3"/>
+      <c r="L75" s="7"/>
       <c r="M75" s="4"/>
       <c r="N75" s="4"/>
     </row>
@@ -3430,7 +3430,7 @@
       <c r="I76">
         <v>74</v>
       </c>
-      <c r="L76" s="1" t="s">
+      <c r="L76" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M76" s="4"/>
@@ -3464,7 +3464,7 @@
       <c r="I77">
         <v>75</v>
       </c>
-      <c r="L77" s="2"/>
+      <c r="L77" s="6"/>
       <c r="M77" s="4"/>
       <c r="N77" s="4"/>
     </row>
@@ -3481,7 +3481,7 @@
       <c r="J78">
         <v>-3</v>
       </c>
-      <c r="L78" s="3"/>
+      <c r="L78" s="7"/>
       <c r="M78" s="4"/>
       <c r="N78" s="4"/>
     </row>
@@ -3513,7 +3513,7 @@
       <c r="I79">
         <v>77</v>
       </c>
-      <c r="L79" s="1" t="s">
+      <c r="L79" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M79" s="4"/>
@@ -3547,7 +3547,7 @@
       <c r="I80">
         <v>78</v>
       </c>
-      <c r="L80" s="2"/>
+      <c r="L80" s="6"/>
       <c r="M80" s="4"/>
       <c r="N80" s="4"/>
     </row>
@@ -3564,7 +3564,7 @@
       <c r="J81">
         <v>-3</v>
       </c>
-      <c r="L81" s="3"/>
+      <c r="L81" s="7"/>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
     </row>
@@ -3596,7 +3596,7 @@
       <c r="I82">
         <v>80</v>
       </c>
-      <c r="L82" s="1" t="s">
+      <c r="L82" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M82" s="4"/>
@@ -3630,7 +3630,7 @@
       <c r="I83">
         <v>81</v>
       </c>
-      <c r="L83" s="2"/>
+      <c r="L83" s="6"/>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
     </row>
@@ -3647,7 +3647,7 @@
       <c r="J84">
         <v>-3</v>
       </c>
-      <c r="L84" s="3"/>
+      <c r="L84" s="7"/>
       <c r="M84" s="4"/>
       <c r="N84" s="4"/>
     </row>
@@ -3679,7 +3679,7 @@
       <c r="I85">
         <v>83</v>
       </c>
-      <c r="L85" s="1" t="s">
+      <c r="L85" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M85" s="4"/>
@@ -3713,7 +3713,7 @@
       <c r="I86">
         <v>84</v>
       </c>
-      <c r="L86" s="2"/>
+      <c r="L86" s="6"/>
       <c r="M86" s="4"/>
       <c r="N86" s="4"/>
     </row>
@@ -3730,7 +3730,7 @@
       <c r="J87">
         <v>-3</v>
       </c>
-      <c r="L87" s="3"/>
+      <c r="L87" s="7"/>
       <c r="M87" s="4"/>
       <c r="N87" s="4"/>
     </row>
@@ -3762,7 +3762,7 @@
       <c r="I88">
         <v>86</v>
       </c>
-      <c r="L88" s="1" t="s">
+      <c r="L88" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M88" s="4"/>
@@ -3796,7 +3796,7 @@
       <c r="I89">
         <v>87</v>
       </c>
-      <c r="L89" s="2"/>
+      <c r="L89" s="6"/>
       <c r="M89" s="4"/>
       <c r="N89" s="4"/>
     </row>
@@ -3813,7 +3813,7 @@
       <c r="J90">
         <v>-3</v>
       </c>
-      <c r="L90" s="3"/>
+      <c r="L90" s="7"/>
       <c r="M90" s="4"/>
       <c r="N90" s="4"/>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="I91">
         <v>89</v>
       </c>
-      <c r="L91" s="1" t="s">
+      <c r="L91" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M91" s="4"/>
@@ -3879,7 +3879,7 @@
       <c r="I92">
         <v>90</v>
       </c>
-      <c r="L92" s="2"/>
+      <c r="L92" s="6"/>
       <c r="M92" s="4"/>
       <c r="N92" s="4"/>
     </row>
@@ -3896,7 +3896,7 @@
       <c r="J93">
         <v>-3</v>
       </c>
-      <c r="L93" s="3"/>
+      <c r="L93" s="7"/>
       <c r="M93" s="4"/>
       <c r="N93" s="4"/>
     </row>
@@ -3975,7 +3975,7 @@
       <c r="H96">
         <v>1</v>
       </c>
-      <c r="I96" s="7">
+      <c r="I96" s="2">
         <v>94</v>
       </c>
       <c r="L96" t="s">
@@ -4015,7 +4015,7 @@
       <c r="L97" t="s">
         <v>35</v>
       </c>
-      <c r="M97" s="5" t="s">
+      <c r="M97" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N97" s="4"/>
@@ -4132,7 +4132,7 @@
       <c r="I101">
         <v>99</v>
       </c>
-      <c r="L101" s="1" t="s">
+      <c r="L101" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M101" s="4"/>
@@ -4166,7 +4166,7 @@
       <c r="I102">
         <v>100</v>
       </c>
-      <c r="L102" s="2"/>
+      <c r="L102" s="6"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
     </row>
@@ -4183,7 +4183,7 @@
       <c r="J103">
         <v>-3</v>
       </c>
-      <c r="L103" s="3"/>
+      <c r="L103" s="7"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
     </row>
@@ -4215,7 +4215,7 @@
       <c r="I104">
         <v>102</v>
       </c>
-      <c r="L104" s="1" t="s">
+      <c r="L104" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M104" s="4"/>
@@ -4249,7 +4249,7 @@
       <c r="I105">
         <v>103</v>
       </c>
-      <c r="L105" s="2"/>
+      <c r="L105" s="6"/>
       <c r="M105" s="4"/>
       <c r="N105" s="4"/>
     </row>
@@ -4266,7 +4266,7 @@
       <c r="J106">
         <v>-3</v>
       </c>
-      <c r="L106" s="3"/>
+      <c r="L106" s="7"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
     </row>
@@ -4298,7 +4298,7 @@
       <c r="I107">
         <v>105</v>
       </c>
-      <c r="L107" s="1" t="s">
+      <c r="L107" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M107" s="4"/>
@@ -4332,7 +4332,7 @@
       <c r="I108">
         <v>106</v>
       </c>
-      <c r="L108" s="2"/>
+      <c r="L108" s="6"/>
       <c r="M108" s="4"/>
       <c r="N108" s="4"/>
     </row>
@@ -4349,7 +4349,7 @@
       <c r="J109">
         <v>-3</v>
       </c>
-      <c r="L109" s="3"/>
+      <c r="L109" s="7"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
     </row>
@@ -4381,7 +4381,7 @@
       <c r="I110">
         <v>108</v>
       </c>
-      <c r="L110" s="1" t="s">
+      <c r="L110" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M110" s="4"/>
@@ -4415,7 +4415,7 @@
       <c r="I111">
         <v>109</v>
       </c>
-      <c r="L111" s="2"/>
+      <c r="L111" s="6"/>
       <c r="M111" s="4"/>
       <c r="N111" s="4"/>
     </row>
@@ -4432,7 +4432,7 @@
       <c r="J112">
         <v>-3</v>
       </c>
-      <c r="L112" s="3"/>
+      <c r="L112" s="7"/>
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
     </row>
@@ -4464,7 +4464,7 @@
       <c r="I113">
         <v>111</v>
       </c>
-      <c r="L113" s="1" t="s">
+      <c r="L113" s="5" t="s">
         <v>30</v>
       </c>
       <c r="M113" s="4"/>
@@ -4498,7 +4498,7 @@
       <c r="I114">
         <v>112</v>
       </c>
-      <c r="L114" s="2"/>
+      <c r="L114" s="6"/>
       <c r="M114" s="4"/>
       <c r="N114" s="4"/>
     </row>
@@ -4515,7 +4515,7 @@
       <c r="J115">
         <v>-3</v>
       </c>
-      <c r="L115" s="3"/>
+      <c r="L115" s="7"/>
       <c r="M115" s="4"/>
       <c r="N115" s="4"/>
     </row>
@@ -4634,7 +4634,7 @@
       <c r="L119" t="s">
         <v>35</v>
       </c>
-      <c r="M119" s="5" t="s">
+      <c r="M119" s="3" t="s">
         <v>38</v>
       </c>
       <c r="N119" s="4"/>
@@ -4652,7 +4652,7 @@
       <c r="L120" t="s">
         <v>36</v>
       </c>
-      <c r="M120" s="5"/>
+      <c r="M120" s="3"/>
       <c r="N120" s="4"/>
     </row>
     <row r="121" spans="1:14" ht="21">
@@ -4683,10 +4683,10 @@
       <c r="I121">
         <v>119</v>
       </c>
-      <c r="L121" s="6" t="s">
+      <c r="L121" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="M121" s="5"/>
+      <c r="M121" s="3"/>
       <c r="N121" s="4"/>
     </row>
     <row r="122" spans="1:14">
@@ -4720,7 +4720,7 @@
       <c r="L122" t="s">
         <v>36</v>
       </c>
-      <c r="M122" s="5"/>
+      <c r="M122" s="3"/>
       <c r="N122" s="4"/>
     </row>
     <row r="123" spans="1:14">
@@ -4754,7 +4754,7 @@
       <c r="L123" t="s">
         <v>36</v>
       </c>
-      <c r="M123" s="5"/>
+      <c r="M123" s="3"/>
       <c r="N123" s="4"/>
     </row>
     <row r="124" spans="1:14">
@@ -4773,7 +4773,7 @@
       <c r="L124" t="s">
         <v>33</v>
       </c>
-      <c r="M124" s="5"/>
+      <c r="M124" s="3"/>
       <c r="N124" s="4"/>
     </row>
     <row r="125" spans="1:14">
@@ -4789,7 +4789,7 @@
       <c r="L125" t="s">
         <v>33</v>
       </c>
-      <c r="M125" s="5"/>
+      <c r="M125" s="3"/>
       <c r="N125" s="4"/>
     </row>
     <row r="126" spans="1:14">
@@ -4808,7 +4808,7 @@
       <c r="L126" t="s">
         <v>33</v>
       </c>
-      <c r="M126" s="5"/>
+      <c r="M126" s="3"/>
       <c r="N126" s="4"/>
     </row>
     <row r="127" spans="1:14">
@@ -4824,7 +4824,7 @@
       <c r="L127" t="s">
         <v>33</v>
       </c>
-      <c r="M127" s="5"/>
+      <c r="M127" s="3"/>
       <c r="N127" s="4"/>
     </row>
     <row r="128" spans="1:14">
@@ -4843,7 +4843,7 @@
       <c r="L128" t="s">
         <v>33</v>
       </c>
-      <c r="M128" s="5"/>
+      <c r="M128" s="3"/>
       <c r="N128" s="4"/>
     </row>
     <row r="129" spans="1:14">
@@ -4859,7 +4859,7 @@
       <c r="L129" t="s">
         <v>33</v>
       </c>
-      <c r="M129" s="5"/>
+      <c r="M129" s="3"/>
       <c r="N129" s="4"/>
     </row>
     <row r="130" spans="1:14">
@@ -4893,7 +4893,7 @@
       <c r="L130" t="s">
         <v>36</v>
       </c>
-      <c r="M130" s="5"/>
+      <c r="M130" s="3"/>
       <c r="N130" s="4"/>
     </row>
     <row r="131" spans="1:14">
@@ -4927,7 +4927,7 @@
       <c r="L131" t="s">
         <v>36</v>
       </c>
-      <c r="M131" s="5"/>
+      <c r="M131" s="3"/>
       <c r="N131" s="4"/>
     </row>
     <row r="132" spans="1:14">
@@ -4961,7 +4961,7 @@
       <c r="L132" t="s">
         <v>36</v>
       </c>
-      <c r="M132" s="5"/>
+      <c r="M132" s="3"/>
       <c r="N132" s="4"/>
     </row>
     <row r="133" spans="1:14">
@@ -4995,7 +4995,7 @@
       <c r="L133" t="s">
         <v>36</v>
       </c>
-      <c r="M133" s="5"/>
+      <c r="M133" s="3"/>
       <c r="N133" s="4"/>
     </row>
     <row r="134" spans="1:14">
@@ -5011,7 +5011,7 @@
       <c r="L134" t="s">
         <v>37</v>
       </c>
-      <c r="M134" s="5"/>
+      <c r="M134" s="3"/>
       <c r="N134" s="4"/>
     </row>
     <row r="135" spans="1:14">
@@ -5039,13 +5039,13 @@
       <c r="H135">
         <v>1</v>
       </c>
-      <c r="I135" s="7">
+      <c r="I135" s="2">
         <v>133</v>
       </c>
       <c r="L135" t="s">
         <v>35</v>
       </c>
-      <c r="M135" s="5"/>
+      <c r="M135" s="3"/>
       <c r="N135" s="4"/>
     </row>
     <row r="136" spans="1:14">
@@ -5107,7 +5107,7 @@
         <v>94</v>
       </c>
       <c r="L138" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="139" spans="1:14">
@@ -5189,10 +5189,10 @@
       <c r="L141" t="s">
         <v>35</v>
       </c>
-      <c r="M141" s="5" t="s">
+      <c r="M141" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N141" s="5"/>
+      <c r="N141" s="3"/>
     </row>
     <row r="142" spans="1:14">
       <c r="A142" t="s">
@@ -5225,8 +5225,8 @@
       <c r="L142" t="s">
         <v>40</v>
       </c>
-      <c r="M142" s="5"/>
-      <c r="N142" s="5"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
     </row>
     <row r="143" spans="1:14">
       <c r="A143" t="s">
@@ -5241,8 +5241,8 @@
       <c r="L143" t="s">
         <v>36</v>
       </c>
-      <c r="M143" s="5"/>
-      <c r="N143" s="5"/>
+      <c r="M143" s="3"/>
+      <c r="N143" s="3"/>
     </row>
     <row r="144" spans="1:14">
       <c r="A144" t="s">
@@ -5275,8 +5275,8 @@
       <c r="L144" t="s">
         <v>36</v>
       </c>
-      <c r="M144" s="5"/>
-      <c r="N144" s="5"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
     </row>
     <row r="145" spans="1:14">
       <c r="A145" t="s">
@@ -5309,8 +5309,8 @@
       <c r="L145" t="s">
         <v>36</v>
       </c>
-      <c r="M145" s="5"/>
-      <c r="N145" s="5"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
     </row>
     <row r="146" spans="1:14">
       <c r="A146" t="s">
@@ -5343,8 +5343,8 @@
       <c r="L146" t="s">
         <v>36</v>
       </c>
-      <c r="M146" s="5"/>
-      <c r="N146" s="5"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
     </row>
     <row r="147" spans="1:14">
       <c r="A147" t="s">
@@ -5377,8 +5377,8 @@
       <c r="L147" t="s">
         <v>36</v>
       </c>
-      <c r="M147" s="5"/>
-      <c r="N147" s="5"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3"/>
     </row>
     <row r="148" spans="1:14">
       <c r="A148" t="s">
@@ -5411,8 +5411,8 @@
       <c r="L148" t="s">
         <v>36</v>
       </c>
-      <c r="M148" s="5"/>
-      <c r="N148" s="5"/>
+      <c r="M148" s="3"/>
+      <c r="N148" s="3"/>
     </row>
     <row r="149" spans="1:14">
       <c r="A149" t="s">
@@ -5445,8 +5445,8 @@
       <c r="L149" t="s">
         <v>36</v>
       </c>
-      <c r="M149" s="5"/>
-      <c r="N149" s="5"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
     </row>
     <row r="150" spans="1:14">
       <c r="A150" t="s">
@@ -5461,8 +5461,8 @@
       <c r="L150" t="s">
         <v>37</v>
       </c>
-      <c r="M150" s="5"/>
-      <c r="N150" s="5"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3"/>
     </row>
     <row r="151" spans="1:14">
       <c r="A151" t="s">
@@ -5489,14 +5489,14 @@
       <c r="H151">
         <v>1</v>
       </c>
-      <c r="I151" s="7">
+      <c r="I151" s="2">
         <v>149</v>
       </c>
       <c r="L151" t="s">
         <v>35</v>
       </c>
-      <c r="M151" s="5"/>
-      <c r="N151" s="5"/>
+      <c r="M151" s="3"/>
+      <c r="N151" s="3"/>
     </row>
     <row r="152" spans="1:14">
       <c r="A152" t="s">
@@ -5557,7 +5557,7 @@
         <v>57</v>
       </c>
       <c r="L154" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="1:14">
@@ -5605,7 +5605,7 @@
         <v>23</v>
       </c>
       <c r="L156" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="157" spans="1:14">
@@ -5639,10 +5639,10 @@
       <c r="L157" t="s">
         <v>35</v>
       </c>
-      <c r="M157" s="5" t="s">
+      <c r="M157" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N157" s="5"/>
+      <c r="N157" s="3"/>
     </row>
     <row r="158" spans="1:14">
       <c r="A158" t="s">
@@ -5675,8 +5675,8 @@
       <c r="L158" t="s">
         <v>40</v>
       </c>
-      <c r="M158" s="5"/>
-      <c r="N158" s="5"/>
+      <c r="M158" s="3"/>
+      <c r="N158" s="3"/>
     </row>
     <row r="159" spans="1:14">
       <c r="A159" t="s">
@@ -5691,8 +5691,8 @@
       <c r="L159" t="s">
         <v>36</v>
       </c>
-      <c r="M159" s="5"/>
-      <c r="N159" s="5"/>
+      <c r="M159" s="3"/>
+      <c r="N159" s="3"/>
     </row>
     <row r="160" spans="1:14">
       <c r="A160" t="s">
@@ -5725,8 +5725,8 @@
       <c r="L160" t="s">
         <v>36</v>
       </c>
-      <c r="M160" s="5"/>
-      <c r="N160" s="5"/>
+      <c r="M160" s="3"/>
+      <c r="N160" s="3"/>
     </row>
     <row r="161" spans="1:15">
       <c r="A161" t="s">
@@ -5759,8 +5759,8 @@
       <c r="L161" t="s">
         <v>36</v>
       </c>
-      <c r="M161" s="5"/>
-      <c r="N161" s="5"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
     </row>
     <row r="162" spans="1:15">
       <c r="A162" t="s">
@@ -5793,8 +5793,8 @@
       <c r="L162" t="s">
         <v>36</v>
       </c>
-      <c r="M162" s="5"/>
-      <c r="N162" s="5"/>
+      <c r="M162" s="3"/>
+      <c r="N162" s="3"/>
     </row>
     <row r="163" spans="1:15">
       <c r="A163" t="s">
@@ -5827,8 +5827,8 @@
       <c r="L163" t="s">
         <v>36</v>
       </c>
-      <c r="M163" s="5"/>
-      <c r="N163" s="5"/>
+      <c r="M163" s="3"/>
+      <c r="N163" s="3"/>
     </row>
     <row r="164" spans="1:15">
       <c r="A164" t="s">
@@ -5861,8 +5861,8 @@
       <c r="L164" t="s">
         <v>36</v>
       </c>
-      <c r="M164" s="5"/>
-      <c r="N164" s="5"/>
+      <c r="M164" s="3"/>
+      <c r="N164" s="3"/>
     </row>
     <row r="165" spans="1:15">
       <c r="A165" t="s">
@@ -5895,8 +5895,8 @@
       <c r="L165" t="s">
         <v>36</v>
       </c>
-      <c r="M165" s="5"/>
-      <c r="N165" s="5"/>
+      <c r="M165" s="3"/>
+      <c r="N165" s="3"/>
     </row>
     <row r="166" spans="1:15">
       <c r="A166" t="s">
@@ -5911,8 +5911,8 @@
       <c r="L166" t="s">
         <v>37</v>
       </c>
-      <c r="M166" s="5"/>
-      <c r="N166" s="5"/>
+      <c r="M166" s="3"/>
+      <c r="N166" s="3"/>
     </row>
     <row r="167" spans="1:15">
       <c r="A167" t="s">
@@ -5939,14 +5939,14 @@
       <c r="H167">
         <v>1</v>
       </c>
-      <c r="I167" s="7">
+      <c r="I167" s="2">
         <v>165</v>
       </c>
       <c r="L167" t="s">
         <v>35</v>
       </c>
-      <c r="M167" s="5"/>
-      <c r="N167" s="5"/>
+      <c r="M167" s="3"/>
+      <c r="N167" s="3"/>
     </row>
     <row r="168" spans="1:15">
       <c r="A168" t="s">
@@ -6118,10 +6118,10 @@
       <c r="L174" t="s">
         <v>35</v>
       </c>
-      <c r="M174" s="5" t="s">
+      <c r="M174" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N174" s="5"/>
+      <c r="N174" s="3"/>
     </row>
     <row r="175" spans="1:15">
       <c r="A175" t="s">
@@ -6154,8 +6154,8 @@
       <c r="L175" t="s">
         <v>40</v>
       </c>
-      <c r="M175" s="5"/>
-      <c r="N175" s="5"/>
+      <c r="M175" s="3"/>
+      <c r="N175" s="3"/>
     </row>
     <row r="176" spans="1:15">
       <c r="A176" t="s">
@@ -6170,8 +6170,8 @@
       <c r="L176" t="s">
         <v>36</v>
       </c>
-      <c r="M176" s="5"/>
-      <c r="N176" s="5"/>
+      <c r="M176" s="3"/>
+      <c r="N176" s="3"/>
     </row>
     <row r="177" spans="1:15">
       <c r="A177" t="s">
@@ -6204,8 +6204,8 @@
       <c r="L177" t="s">
         <v>36</v>
       </c>
-      <c r="M177" s="5"/>
-      <c r="N177" s="5"/>
+      <c r="M177" s="3"/>
+      <c r="N177" s="3"/>
     </row>
     <row r="178" spans="1:15">
       <c r="A178" t="s">
@@ -6238,8 +6238,8 @@
       <c r="L178" t="s">
         <v>36</v>
       </c>
-      <c r="M178" s="5"/>
-      <c r="N178" s="5"/>
+      <c r="M178" s="3"/>
+      <c r="N178" s="3"/>
     </row>
     <row r="179" spans="1:15">
       <c r="A179" t="s">
@@ -6272,8 +6272,8 @@
       <c r="L179" t="s">
         <v>36</v>
       </c>
-      <c r="M179" s="5"/>
-      <c r="N179" s="5"/>
+      <c r="M179" s="3"/>
+      <c r="N179" s="3"/>
     </row>
     <row r="180" spans="1:15">
       <c r="A180" t="s">
@@ -6306,8 +6306,8 @@
       <c r="L180" t="s">
         <v>36</v>
       </c>
-      <c r="M180" s="5"/>
-      <c r="N180" s="5"/>
+      <c r="M180" s="3"/>
+      <c r="N180" s="3"/>
     </row>
     <row r="181" spans="1:15">
       <c r="A181" t="s">
@@ -6340,8 +6340,8 @@
       <c r="L181" t="s">
         <v>36</v>
       </c>
-      <c r="M181" s="5"/>
-      <c r="N181" s="5"/>
+      <c r="M181" s="3"/>
+      <c r="N181" s="3"/>
     </row>
     <row r="182" spans="1:15">
       <c r="A182" t="s">
@@ -6374,8 +6374,8 @@
       <c r="L182" t="s">
         <v>36</v>
       </c>
-      <c r="M182" s="5"/>
-      <c r="N182" s="5"/>
+      <c r="M182" s="3"/>
+      <c r="N182" s="3"/>
     </row>
     <row r="183" spans="1:15">
       <c r="A183" t="s">
@@ -6390,8 +6390,8 @@
       <c r="L183" t="s">
         <v>37</v>
       </c>
-      <c r="M183" s="5"/>
-      <c r="N183" s="5"/>
+      <c r="M183" s="3"/>
+      <c r="N183" s="3"/>
     </row>
     <row r="184" spans="1:15">
       <c r="A184" t="s">
@@ -6418,14 +6418,14 @@
       <c r="H184">
         <v>1</v>
       </c>
-      <c r="I184" s="7">
+      <c r="I184" s="2">
         <v>182</v>
       </c>
       <c r="L184" t="s">
         <v>35</v>
       </c>
-      <c r="M184" s="5"/>
-      <c r="N184" s="5"/>
+      <c r="M184" s="3"/>
+      <c r="N184" s="3"/>
     </row>
     <row r="185" spans="1:15">
       <c r="A185" t="s">
@@ -6597,10 +6597,10 @@
       <c r="L191" t="s">
         <v>35</v>
       </c>
-      <c r="M191" s="5" t="s">
+      <c r="M191" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N191" s="5"/>
+      <c r="N191" s="3"/>
     </row>
     <row r="192" spans="1:15">
       <c r="A192" t="s">
@@ -6633,8 +6633,8 @@
       <c r="L192" t="s">
         <v>40</v>
       </c>
-      <c r="M192" s="5"/>
-      <c r="N192" s="5"/>
+      <c r="M192" s="3"/>
+      <c r="N192" s="3"/>
     </row>
     <row r="193" spans="1:15">
       <c r="A193" t="s">
@@ -6649,8 +6649,8 @@
       <c r="L193" t="s">
         <v>36</v>
       </c>
-      <c r="M193" s="5"/>
-      <c r="N193" s="5"/>
+      <c r="M193" s="3"/>
+      <c r="N193" s="3"/>
     </row>
     <row r="194" spans="1:15">
       <c r="A194" t="s">
@@ -6683,8 +6683,8 @@
       <c r="L194" t="s">
         <v>36</v>
       </c>
-      <c r="M194" s="5"/>
-      <c r="N194" s="5"/>
+      <c r="M194" s="3"/>
+      <c r="N194" s="3"/>
     </row>
     <row r="195" spans="1:15">
       <c r="A195" t="s">
@@ -6717,8 +6717,8 @@
       <c r="L195" t="s">
         <v>36</v>
       </c>
-      <c r="M195" s="5"/>
-      <c r="N195" s="5"/>
+      <c r="M195" s="3"/>
+      <c r="N195" s="3"/>
     </row>
     <row r="196" spans="1:15">
       <c r="A196" t="s">
@@ -6751,8 +6751,8 @@
       <c r="L196" t="s">
         <v>36</v>
       </c>
-      <c r="M196" s="5"/>
-      <c r="N196" s="5"/>
+      <c r="M196" s="3"/>
+      <c r="N196" s="3"/>
     </row>
     <row r="197" spans="1:15">
       <c r="A197" t="s">
@@ -6785,8 +6785,8 @@
       <c r="L197" t="s">
         <v>36</v>
       </c>
-      <c r="M197" s="5"/>
-      <c r="N197" s="5"/>
+      <c r="M197" s="3"/>
+      <c r="N197" s="3"/>
     </row>
     <row r="198" spans="1:15">
       <c r="A198" t="s">
@@ -6819,8 +6819,8 @@
       <c r="L198" t="s">
         <v>36</v>
       </c>
-      <c r="M198" s="5"/>
-      <c r="N198" s="5"/>
+      <c r="M198" s="3"/>
+      <c r="N198" s="3"/>
     </row>
     <row r="199" spans="1:15">
       <c r="A199" t="s">
@@ -6853,8 +6853,8 @@
       <c r="L199" t="s">
         <v>36</v>
       </c>
-      <c r="M199" s="5"/>
-      <c r="N199" s="5"/>
+      <c r="M199" s="3"/>
+      <c r="N199" s="3"/>
     </row>
     <row r="200" spans="1:15">
       <c r="A200" t="s">
@@ -6869,8 +6869,8 @@
       <c r="L200" t="s">
         <v>37</v>
       </c>
-      <c r="M200" s="5"/>
-      <c r="N200" s="5"/>
+      <c r="M200" s="3"/>
+      <c r="N200" s="3"/>
     </row>
     <row r="201" spans="1:15">
       <c r="A201" t="s">
@@ -6903,8 +6903,8 @@
       <c r="L201" t="s">
         <v>35</v>
       </c>
-      <c r="M201" s="5"/>
-      <c r="N201" s="5"/>
+      <c r="M201" s="3"/>
+      <c r="N201" s="3"/>
     </row>
     <row r="202" spans="1:15">
       <c r="A202" t="s">
@@ -6985,23 +6985,42 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="M174:N184"/>
-    <mergeCell ref="L185:N187"/>
-    <mergeCell ref="L189:N189"/>
-    <mergeCell ref="M191:N201"/>
-    <mergeCell ref="L202:N204"/>
+    <mergeCell ref="L48:L50"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="L27:L29"/>
+    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="L91:L93"/>
+    <mergeCell ref="L51:L53"/>
+    <mergeCell ref="L54:L56"/>
+    <mergeCell ref="L64:L66"/>
+    <mergeCell ref="L67:L69"/>
+    <mergeCell ref="L70:L72"/>
+    <mergeCell ref="L73:L75"/>
+    <mergeCell ref="L76:L78"/>
+    <mergeCell ref="L79:L81"/>
+    <mergeCell ref="L82:L84"/>
+    <mergeCell ref="L85:L87"/>
+    <mergeCell ref="L88:L90"/>
+    <mergeCell ref="L155:N155"/>
+    <mergeCell ref="M157:N167"/>
+    <mergeCell ref="L168:N170"/>
+    <mergeCell ref="L172:N172"/>
+    <mergeCell ref="L136:N137"/>
+    <mergeCell ref="L139:N139"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:N135"/>
     <mergeCell ref="L152:N153"/>
     <mergeCell ref="M141:N151"/>
-    <mergeCell ref="L155:N155"/>
-    <mergeCell ref="M157:N167"/>
-    <mergeCell ref="L168:N170"/>
-    <mergeCell ref="L172:N172"/>
-    <mergeCell ref="L136:N137"/>
     <mergeCell ref="M119:M135"/>
-    <mergeCell ref="L139:N139"/>
     <mergeCell ref="L101:L103"/>
     <mergeCell ref="L104:L106"/>
     <mergeCell ref="L107:L109"/>
@@ -7012,30 +7031,11 @@
     <mergeCell ref="M23:M59"/>
     <mergeCell ref="M60:M96"/>
     <mergeCell ref="M97:M118"/>
-    <mergeCell ref="L76:L78"/>
-    <mergeCell ref="L79:L81"/>
-    <mergeCell ref="L82:L84"/>
-    <mergeCell ref="L85:L87"/>
-    <mergeCell ref="L88:L90"/>
-    <mergeCell ref="L91:L93"/>
-    <mergeCell ref="L51:L53"/>
-    <mergeCell ref="L54:L56"/>
-    <mergeCell ref="L64:L66"/>
-    <mergeCell ref="L67:L69"/>
-    <mergeCell ref="L70:L72"/>
-    <mergeCell ref="L73:L75"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L36:L38"/>
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="L45:L47"/>
-    <mergeCell ref="L48:L50"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="L30:L32"/>
+    <mergeCell ref="M174:N184"/>
+    <mergeCell ref="L185:N187"/>
+    <mergeCell ref="L189:N189"/>
+    <mergeCell ref="M191:N201"/>
+    <mergeCell ref="L202:N204"/>
   </mergeCells>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>